<commit_message>
updated lecture slides for chpater 3.
</commit_message>
<xml_diff>
--- a/stat4110-schedule.xlsx
+++ b/stat4110-schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliPe\Documents\GitHub Repositories\Ali-Raisolsadat.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7F00C18-188D-44FD-9FAE-51C1713D743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1BE270-E9C9-41EC-B137-BA3CC8CE9A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E80023EF-6428-48D2-ABA1-FC32C6C952F1}"/>
   </bookViews>
@@ -95,12 +95,6 @@
     <t>Apr 6–10</t>
   </si>
   <si>
-    <t>Final Project Presentations (Groups 1 &amp; 2)</t>
-  </si>
-  <si>
-    <t>Final Project Presentations (Groups 3 &amp; 4)</t>
-  </si>
-  <si>
     <t>—</t>
   </si>
   <si>
@@ -128,21 +122,12 @@
     <t>Lecture 4 (Chapter 2)</t>
   </si>
   <si>
-    <t>Quiz 1 (Chapter 1)</t>
-  </si>
-  <si>
-    <t>Quiz 3 (Chapter 3)</t>
-  </si>
-  <si>
     <t>Lecture 1 (Chapter 4)</t>
   </si>
   <si>
     <t>Lecture 2 (Chapter 4)</t>
   </si>
   <si>
-    <t>Quiz 4 (Chapter 4)</t>
-  </si>
-  <si>
     <t>Lecture 1 (Chapter 5)</t>
   </si>
   <si>
@@ -200,13 +185,28 @@
     <t>Assignment 1 Due Feb 15</t>
   </si>
   <si>
-    <t>Assignment 2 Due Mar 15</t>
-  </si>
-  <si>
     <t>Final Project Report Due Apr 17</t>
   </si>
   <si>
-    <t>Deliverable 1: Project Summary &amp; Team Plan Due Mar 1, Assignment 2 Published Mar 1</t>
+    <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 4 </t>
+  </si>
+  <si>
+    <t>Assignment 2 Review</t>
+  </si>
+  <si>
+    <t>Assignment 2 Due Mar 20</t>
+  </si>
+  <si>
+    <t>Project Summary &amp; Team Plan Due Mar 1, Assignment 2 Published Mar 1</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
     <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,16 +631,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,16 +648,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,16 +665,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,16 +682,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -699,16 +699,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +725,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -733,30 +733,30 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>38</v>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>56</v>
@@ -766,17 +766,17 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,84 +784,84 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>34</v>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>36</v>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated the class schedule
</commit_message>
<xml_diff>
--- a/stat4110-schedule.xlsx
+++ b/stat4110-schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliPe\Documents\GitHub Repositories\Ali-Raisolsadat.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1BE270-E9C9-41EC-B137-BA3CC8CE9A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E47C69-9E59-48D3-A507-0D0AF6110BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E80023EF-6428-48D2-ABA1-FC32C6C952F1}"/>
+    <workbookView xWindow="9270" yWindow="675" windowWidth="16995" windowHeight="14805" xr2:uid="{E80023EF-6428-48D2-ABA1-FC32C6C952F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Week (Mon–Fri)</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Project Summary &amp; Team Plan Due Mar 1, Assignment 2 Published Mar 1</t>
+  </si>
+  <si>
+    <t>Lecture 0 (Chapter 1)</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41919B0E-E49A-45AF-B9D7-9D41FA577667}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -654,7 +660,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -664,14 +670,14 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
@@ -681,14 +687,14 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>51</v>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>47</v>
@@ -699,13 +705,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
@@ -733,13 +739,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
@@ -749,14 +755,14 @@
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>50</v>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>56</v>
@@ -766,14 +772,14 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -784,13 +790,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>55</v>
@@ -801,13 +807,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>19</v>
@@ -817,14 +823,14 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
@@ -834,14 +840,14 @@
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>19</v>
@@ -852,10 +858,10 @@
         <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>
@@ -870,9 +876,12 @@
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+    </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
@@ -944,6 +953,7 @@
       <c r="C31" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="79" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>